<commit_message>
Trace for Reset price working adequately to debug the process itself
</commit_message>
<xml_diff>
--- a/supplementary/SR EPR/Equal Profit Rate updated.xlsx
+++ b/supplementary/SR EPR/Equal Profit Rate updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\Documents\My Works\REPOS\simulation-api\supplementary\SR EPR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\freeman\Documents\+ADDITIONS\CANADA AND MEXICO\REPOS\simulation-api\supplementary\SR EPR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F6898D-D0D7-4496-BC93-7DE8B3D4BE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8165FD-641A-4CEE-B8AA-2CA10BF77762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" tabRatio="898" activeTab="2" xr2:uid="{17F4EA5B-BF8B-4E69-A145-5100AE639A53}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" tabRatio="898" activeTab="2" xr2:uid="{17F4EA5B-BF8B-4E69-A145-5100AE639A53}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbitrary Prices" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={9BE8C193-1924-4DDF-9910-1F8730C80D69}</author>
+  </authors>
+  <commentList>
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{9BE8C193-1924-4DDF-9910-1F8730C80D69}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    We assume that the price of labour power remains the same, for the purpose of demonstration. In other words, the real wage rises</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="53">
   <si>
@@ -196,7 +214,7 @@
     <t>Output unit prices</t>
   </si>
   <si>
-    <t>NOT RIGHT YET!</t>
+    <t>RIGHT</t>
   </si>
 </sst>
 </file>
@@ -207,7 +225,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +260,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -335,6 +359,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Alan Freeman" id="{08795379-4F08-4EF7-951D-E9541EE6D052}" userId="S::Alan.Freeman@umanitoba.ca::ee058598-dfd7-467d-a2c7-cca2212144aa" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -652,6 +682,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C21" dT="2024-11-26T16:09:58.64" personId="{08795379-4F08-4EF7-951D-E9541EE6D052}" id="{9BE8C193-1924-4DDF-9910-1F8730C80D69}">
+    <text>We assume that the price of labour power remains the same, for the purpose of demonstration. In other words, the real wage rises</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65849331-C705-4E9C-89F1-B53946C8B795}">
   <dimension ref="B1:M32"/>
@@ -1716,11 +1754,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5E4ACA-834C-4FF0-AEE9-90A7FB61F326}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5E4ACA-834C-4FF0-AEE9-90A7FB61F326}">
   <dimension ref="B1:Y24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21:Y21"/>
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2274,31 +2312,31 @@
         <v>4.5714285714285712</v>
       </c>
       <c r="E22" s="3">
-        <f>F$9*C$23</f>
-        <v>6.8571428571428568</v>
+        <f>F$9*C$21</f>
+        <v>4</v>
       </c>
       <c r="F22" s="3">
         <f>D22+E22</f>
-        <v>11.428571428571427</v>
+        <v>8.5714285714285712</v>
       </c>
       <c r="G22" s="3">
         <f>F$9-E22</f>
-        <v>1.1428571428571432</v>
+        <v>4</v>
       </c>
       <c r="H22" s="5">
         <f>F22+G22</f>
-        <v>12.571428571428569</v>
+        <v>12.571428571428571</v>
       </c>
       <c r="J22" s="15">
         <f>G22/F22</f>
-        <v>0.10000000000000005</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="K22" s="7">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="L22" s="16">
-        <f>E$9*C$16</f>
-        <v>4</v>
+        <f>E$9*C$22</f>
+        <v>4.5714285714285712</v>
       </c>
       <c r="M22" s="16">
         <f>F$9*C21</f>
@@ -2306,34 +2344,34 @@
       </c>
       <c r="N22" s="17">
         <f>L22+M22</f>
-        <v>8</v>
+        <v>8.5714285714285712</v>
       </c>
       <c r="O22" s="16">
         <f>G$9*K22</f>
-        <v>12</v>
+        <v>14.399999999999999</v>
       </c>
       <c r="P22" t="s">
         <v>19</v>
       </c>
       <c r="Q22" s="3">
         <f>O24</f>
-        <v>24</v>
+        <v>25.2</v>
       </c>
       <c r="R22" s="5">
-        <f>K22/Q$18</f>
-        <v>0.95238095238095233</v>
+        <f>K22/Q$24</f>
+        <v>1.2244897959183674</v>
       </c>
       <c r="S22" s="5">
         <f>G$9*R22</f>
-        <v>11.428571428571427</v>
+        <v>14.693877551020408</v>
       </c>
       <c r="T22" s="5">
         <f>S22-N22</f>
-        <v>3.428571428571427</v>
+        <v>6.1224489795918373</v>
       </c>
       <c r="U22" s="3">
         <f>T22/N22</f>
-        <v>0.42857142857142838</v>
+        <v>0.71428571428571441</v>
       </c>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.4">
@@ -2349,16 +2387,16 @@
         <v>9.1428571428571423</v>
       </c>
       <c r="E23" s="3">
-        <f>F$10*C$23</f>
-        <v>3.4285714285714284</v>
+        <f>F$10*C$21</f>
+        <v>2</v>
       </c>
       <c r="F23" s="3">
         <f>D23+E23</f>
-        <v>12.571428571428571</v>
+        <v>11.142857142857142</v>
       </c>
       <c r="G23" s="3">
         <f>F$10-E23</f>
-        <v>0.57142857142857162</v>
+        <v>2</v>
       </c>
       <c r="H23" s="5">
         <f>F23+G23</f>
@@ -2366,14 +2404,14 @@
       </c>
       <c r="J23" s="15">
         <f>G23/F23</f>
-        <v>4.545454545454547E-2</v>
+        <v>0.17948717948717949</v>
       </c>
       <c r="K23" s="7">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="L23" s="16">
-        <f>E$10*C$16</f>
-        <v>8</v>
+        <f>E$10*C$22</f>
+        <v>9.1428571428571423</v>
       </c>
       <c r="M23" s="16">
         <f>F$10*K21</f>
@@ -2381,34 +2419,34 @@
       </c>
       <c r="N23" s="17">
         <f>L23+M23</f>
-        <v>10</v>
+        <v>11.142857142857142</v>
       </c>
       <c r="O23" s="16">
         <f>G$10*K23</f>
-        <v>12</v>
+        <v>10.8</v>
       </c>
       <c r="P23" t="s">
         <v>18</v>
       </c>
       <c r="Q23" s="5">
         <f>H24</f>
-        <v>25.714285714285712</v>
+        <v>25.714285714285715</v>
       </c>
       <c r="R23" s="5">
-        <f>K23/Q$18</f>
-        <v>0.95238095238095233</v>
+        <f>K23/Q$24</f>
+        <v>0.91836734693877553</v>
       </c>
       <c r="S23" s="5">
         <f>G$10*R23</f>
-        <v>11.428571428571427</v>
+        <v>11.020408163265307</v>
       </c>
       <c r="T23" s="5">
         <f>S23-N23</f>
-        <v>1.428571428571427</v>
+        <v>-0.12244897959183554</v>
       </c>
       <c r="U23" s="3">
         <f>T23/N23</f>
-        <v>0.14285714285714271</v>
+        <v>-1.0989010989010882E-2</v>
       </c>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.4">
@@ -2421,28 +2459,28 @@
       </c>
       <c r="E24" s="5">
         <f>E23+E22</f>
-        <v>10.285714285714285</v>
+        <v>6</v>
       </c>
       <c r="F24" s="5">
         <f>F23+F22</f>
-        <v>24</v>
+        <v>19.714285714285715</v>
       </c>
       <c r="G24" s="9">
         <f>G23+G22</f>
-        <v>1.7142857142857149</v>
+        <v>6</v>
       </c>
       <c r="H24">
         <f>H23+H22</f>
-        <v>25.714285714285712</v>
+        <v>25.714285714285715</v>
       </c>
       <c r="J24" s="15">
         <f>G24/F24</f>
-        <v>7.1428571428571452E-2</v>
+        <v>0.30434782608695649</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="17">
         <f>L22+L23</f>
-        <v>12</v>
+        <v>13.714285714285714</v>
       </c>
       <c r="M24" s="17">
         <f>M22+M23</f>
@@ -2450,30 +2488,30 @@
       </c>
       <c r="N24" s="17">
         <f>N22+N23</f>
-        <v>18</v>
+        <v>19.714285714285715</v>
       </c>
       <c r="O24" s="17">
         <f>O22+O23</f>
-        <v>24</v>
+        <v>25.2</v>
       </c>
       <c r="P24" t="s">
         <v>13</v>
       </c>
       <c r="Q24" s="5">
         <f>Q22/Q23</f>
-        <v>0.93333333333333346</v>
+        <v>0.98</v>
       </c>
       <c r="S24" s="3">
         <f>S22+S23</f>
-        <v>22.857142857142854</v>
+        <v>25.714285714285715</v>
       </c>
       <c r="T24" s="9">
         <f>T22+T23</f>
-        <v>4.8571428571428541</v>
+        <v>6.0000000000000018</v>
       </c>
       <c r="U24" s="3">
         <f>T24/N24</f>
-        <v>0.26984126984126966</v>
+        <v>0.3043478260869566</v>
       </c>
     </row>
   </sheetData>
@@ -2483,5 +2521,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed setprice single; corrected class stock requirement in simulation 5
</commit_message>
<xml_diff>
--- a/supplementary/SR EPR/Equal Profit Rate updated.xlsx
+++ b/supplementary/SR EPR/Equal Profit Rate updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28407"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\freeman\Documents\+ADDITIONS\CANADA AND MEXICO\REPOS\simulation-api\supplementary\SR EPR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\Documents\My Works\REPOS\simulation-api\supplementary\SR EPR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8165FD-641A-4CEE-B8AA-2CA10BF77762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D8B095-273E-4D31-B444-24EB463E7C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" tabRatio="898" activeTab="2" xr2:uid="{17F4EA5B-BF8B-4E69-A145-5100AE639A53}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" tabRatio="898" activeTab="2" xr2:uid="{17F4EA5B-BF8B-4E69-A145-5100AE639A53}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbitrary Prices" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="54">
   <si>
     <t>C</t>
   </si>
@@ -214,18 +214,22 @@
     <t>Output unit prices</t>
   </si>
   <si>
-    <t>RIGHT</t>
+    <t>Un-normalised Unit Prices</t>
+  </si>
+  <si>
+    <t>Normalised Unit Prices</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,22 +257,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,12 +268,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +286,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -329,15 +313,20 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -359,6 +348,200 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>182337</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>73478</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>587829</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>168728</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7823620C-45AC-5037-4CD8-CF7F742F2B85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4776108" y="6887935"/>
+          <a:ext cx="6664778" cy="280307"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" kern="1200"/>
+            <a:t>The normalised profit rate (with total price=total value) should</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" kern="1200" baseline="0"/>
+            <a:t> be</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" kern="1200"/>
+            <a:t> equal to the surplus value (in the absence of stocks)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>321129</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>182337</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10D49D79-5E3D-FE87-16A9-2AECE65A9D96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4267200" y="6596743"/>
+          <a:ext cx="508908" cy="431346"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>587829</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>386443</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFF3C4D6-D548-BA5F-781A-C719DF20187E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11440886" y="6596743"/>
+          <a:ext cx="451757" cy="431346"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1218,18 +1401,18 @@
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="I31" s="18" t="s">
+      <c r="I31" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
     </row>
     <row r="32" spans="2:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="I32" s="19" t="s">
+      <c r="I32" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1755,10 +1938,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5E4ACA-834C-4FF0-AEE9-90A7FB61F326}">
-  <dimension ref="B1:Y24"/>
+  <dimension ref="B1:Y26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1767,15 +1950,17 @@
     <col min="2" max="2" width="13.53515625" customWidth="1"/>
     <col min="3" max="3" width="7.69140625" customWidth="1"/>
     <col min="4" max="4" width="7.61328125" customWidth="1"/>
-    <col min="5" max="5" width="6.4609375" customWidth="1"/>
-    <col min="6" max="6" width="6.4609375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.84375" customWidth="1"/>
-    <col min="8" max="8" width="7.3046875" customWidth="1"/>
+    <col min="5" max="5" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.15234375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.84375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.4609375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.53515625" customWidth="1"/>
-    <col min="11" max="11" width="9.69140625" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.69140625" customWidth="1"/>
-    <col min="13" max="14" width="6.4609375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.53515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.3828125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.3046875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1888,28 +2073,28 @@
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="11">
-        <v>4</v>
-      </c>
-      <c r="F9" s="5">
-        <v>8</v>
-      </c>
-      <c r="G9" s="11">
-        <v>12</v>
+      <c r="E9" s="18">
+        <v>4000</v>
+      </c>
+      <c r="F9" s="19">
+        <v>8000</v>
+      </c>
+      <c r="G9" s="18">
+        <v>12000</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="3">
-        <v>8</v>
-      </c>
-      <c r="F10" s="5">
-        <v>4</v>
-      </c>
-      <c r="G10" s="7">
-        <v>12</v>
+      <c r="E10" s="20">
+        <v>8000</v>
+      </c>
+      <c r="F10" s="19">
+        <v>4000</v>
+      </c>
+      <c r="G10" s="21">
+        <v>12000</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -1917,14 +2102,15 @@
       <c r="D11" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="20">
         <f>E9+E10</f>
-        <v>12</v>
-      </c>
-      <c r="F11" s="3">
+        <v>12000</v>
+      </c>
+      <c r="F11" s="20">
         <f>F9+F10</f>
-        <v>12</v>
-      </c>
+        <v>12000</v>
+      </c>
+      <c r="G11" s="19"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.4">
@@ -1936,12 +2122,12 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="R13" s="18" t="s">
+      <c r="R13" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
       <c r="V13" s="8"/>
       <c r="W13" s="8"/>
       <c r="X13" s="8"/>
@@ -2021,25 +2207,25 @@
       <c r="C16" s="7">
         <v>1</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="20">
         <f>E$9*C$16</f>
-        <v>4</v>
-      </c>
-      <c r="E16" s="3">
+        <v>4000</v>
+      </c>
+      <c r="E16" s="20">
         <f>F$9*C$15</f>
-        <v>4</v>
-      </c>
-      <c r="F16" s="3">
+        <v>4000</v>
+      </c>
+      <c r="F16" s="20">
         <f>D16+E16</f>
-        <v>8</v>
-      </c>
-      <c r="G16" s="3">
+        <v>8000</v>
+      </c>
+      <c r="G16" s="20">
         <f>F$9-E16</f>
-        <v>4</v>
-      </c>
-      <c r="H16" s="5">
+        <v>4000</v>
+      </c>
+      <c r="H16" s="19">
         <f>F16+G16</f>
-        <v>12</v>
+        <v>12000</v>
       </c>
       <c r="J16" s="15">
         <f>G16/F16</f>
@@ -2048,72 +2234,72 @@
       <c r="K16" s="7">
         <v>1.2</v>
       </c>
-      <c r="L16" s="16">
+      <c r="L16" s="23">
         <f>E$9*C$16</f>
-        <v>4</v>
-      </c>
-      <c r="M16" s="16">
+        <v>4000</v>
+      </c>
+      <c r="M16" s="23">
         <f>F$9*C15</f>
-        <v>4</v>
-      </c>
-      <c r="N16" s="17">
+        <v>4000</v>
+      </c>
+      <c r="N16" s="24">
         <f>L16+M16</f>
-        <v>8</v>
-      </c>
-      <c r="O16" s="16">
+        <v>8000</v>
+      </c>
+      <c r="O16" s="23">
         <f>G$9*K16</f>
-        <v>14.399999999999999</v>
+        <v>14400</v>
       </c>
       <c r="P16" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="Q16" s="20">
         <f>O18</f>
-        <v>25.2</v>
+        <v>25200</v>
       </c>
       <c r="R16" s="5">
         <f>K16/Q$18</f>
         <v>1.1428571428571428</v>
       </c>
-      <c r="S16" s="5">
+      <c r="S16" s="19">
         <f>G$9*R16</f>
-        <v>13.714285714285714</v>
-      </c>
-      <c r="T16" s="5">
+        <v>13714.285714285714</v>
+      </c>
+      <c r="T16" s="19">
         <f>S16-N16</f>
-        <v>5.7142857142857135</v>
+        <v>5714.2857142857138</v>
       </c>
       <c r="U16" s="3">
         <f>T16/N16</f>
         <v>0.71428571428571419</v>
       </c>
     </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="20">
         <f>E$10*C$16</f>
-        <v>8</v>
-      </c>
-      <c r="E17" s="3">
+        <v>8000</v>
+      </c>
+      <c r="E17" s="20">
         <f>F$10*C$15</f>
-        <v>2</v>
-      </c>
-      <c r="F17" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F17" s="20">
         <f>D17+E17</f>
-        <v>10</v>
-      </c>
-      <c r="G17" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G17" s="20">
         <f>F$10-E17</f>
-        <v>2</v>
-      </c>
-      <c r="H17" s="5">
+        <v>2000</v>
+      </c>
+      <c r="H17" s="19">
         <f>F17+G17</f>
-        <v>12</v>
+        <v>12000</v>
       </c>
       <c r="J17" s="15">
         <f>G17/F17</f>
@@ -2122,90 +2308,90 @@
       <c r="K17" s="7">
         <v>0.9</v>
       </c>
-      <c r="L17" s="16">
+      <c r="L17" s="23">
         <f>E$10*C$16</f>
-        <v>8</v>
-      </c>
-      <c r="M17" s="16">
+        <v>8000</v>
+      </c>
+      <c r="M17" s="23">
         <f>F$10*K15</f>
-        <v>2</v>
-      </c>
-      <c r="N17" s="17">
+        <v>2000</v>
+      </c>
+      <c r="N17" s="24">
         <f>L17+M17</f>
-        <v>10</v>
-      </c>
-      <c r="O17" s="16">
+        <v>10000</v>
+      </c>
+      <c r="O17" s="23">
         <f>G$10*K17</f>
-        <v>10.8</v>
+        <v>10800</v>
       </c>
       <c r="P17" t="s">
         <v>18</v>
       </c>
-      <c r="Q17" s="5">
+      <c r="Q17" s="19">
         <f>H18</f>
-        <v>24</v>
+        <v>24000</v>
       </c>
       <c r="R17" s="5">
         <f>K17/Q$18</f>
         <v>0.8571428571428571</v>
       </c>
-      <c r="S17" s="5">
+      <c r="S17" s="19">
         <f>G$10*R17</f>
-        <v>10.285714285714285</v>
-      </c>
-      <c r="T17" s="5">
+        <v>10285.714285714284</v>
+      </c>
+      <c r="T17" s="19">
         <f>S17-N17</f>
-        <v>0.2857142857142847</v>
+        <v>285.71428571428442</v>
       </c>
       <c r="U17" s="3">
         <f>T17/N17</f>
-        <v>2.857142857142847E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.4">
+        <v>2.8571428571428442E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="19">
         <f>D17+D16</f>
-        <v>12</v>
-      </c>
-      <c r="E18" s="5">
+        <v>12000</v>
+      </c>
+      <c r="E18" s="19">
         <f>E17+E16</f>
-        <v>6</v>
-      </c>
-      <c r="F18" s="5">
+        <v>6000</v>
+      </c>
+      <c r="F18" s="19">
         <f>F17+F16</f>
-        <v>18</v>
-      </c>
-      <c r="G18" s="9">
+        <v>18000</v>
+      </c>
+      <c r="G18" s="22">
         <f>G17+G16</f>
-        <v>6</v>
-      </c>
-      <c r="H18">
+        <v>6000</v>
+      </c>
+      <c r="H18" s="19">
         <f>H17+H16</f>
-        <v>24</v>
+        <v>24000</v>
       </c>
       <c r="J18" s="15">
         <f>G18/F18</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="L18" s="17">
+      <c r="L18" s="24">
         <f>L16+L17</f>
-        <v>12</v>
-      </c>
-      <c r="M18" s="17">
+        <v>12000</v>
+      </c>
+      <c r="M18" s="24">
         <f>M16+M17</f>
-        <v>6</v>
-      </c>
-      <c r="N18" s="17">
+        <v>6000</v>
+      </c>
+      <c r="N18" s="24">
         <f>N16+N17</f>
-        <v>18</v>
-      </c>
-      <c r="O18" s="17">
+        <v>18000</v>
+      </c>
+      <c r="O18" s="24">
         <f>O16+O17</f>
-        <v>25.2</v>
+        <v>25200</v>
       </c>
       <c r="P18" t="s">
         <v>13</v>
@@ -2214,20 +2400,20 @@
         <f>Q16/Q17</f>
         <v>1.05</v>
       </c>
-      <c r="S18" s="3">
+      <c r="S18" s="20">
         <f>S16+S17</f>
-        <v>24</v>
-      </c>
-      <c r="T18" s="9">
+        <v>24000</v>
+      </c>
+      <c r="T18" s="22">
         <f>T16+T17</f>
-        <v>5.9999999999999982</v>
+        <v>5999.9999999999982</v>
       </c>
       <c r="U18" s="3">
         <f>T18/N18</f>
         <v>0.33333333333333326</v>
       </c>
     </row>
-    <row r="20" spans="2:25" ht="37.299999999999997" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:21" ht="82.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C20" s="13" t="s">
         <v>42</v>
       </c>
@@ -2250,7 +2436,7 @@
         <v>12</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>48</v>
@@ -2265,7 +2451,7 @@
         <v>46</v>
       </c>
       <c r="R20" s="13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="S20" s="8" t="s">
         <v>15</v>
@@ -2277,7 +2463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -2293,13 +2479,8 @@
         <f>K21</f>
         <v>0.5</v>
       </c>
-      <c r="W21" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="X21" s="20"/>
-      <c r="Y21" s="20"/>
-    </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>4</v>
       </c>
@@ -2307,74 +2488,74 @@
         <f>R16</f>
         <v>1.1428571428571428</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="20">
         <f>E$9*C$22</f>
-        <v>4.5714285714285712</v>
-      </c>
-      <c r="E22" s="3">
+        <v>4571.4285714285716</v>
+      </c>
+      <c r="E22" s="20">
         <f>F$9*C$21</f>
-        <v>4</v>
-      </c>
-      <c r="F22" s="3">
+        <v>4000</v>
+      </c>
+      <c r="F22" s="20">
         <f>D22+E22</f>
-        <v>8.5714285714285712</v>
-      </c>
-      <c r="G22" s="3">
+        <v>8571.4285714285725</v>
+      </c>
+      <c r="G22" s="20">
         <f>F$9-E22</f>
-        <v>4</v>
-      </c>
-      <c r="H22" s="5">
+        <v>4000</v>
+      </c>
+      <c r="H22" s="19">
         <f>F22+G22</f>
-        <v>12.571428571428571</v>
+        <v>12571.428571428572</v>
       </c>
       <c r="J22" s="15">
         <f>G22/F22</f>
-        <v>0.46666666666666667</v>
+        <v>0.46666666666666662</v>
       </c>
       <c r="K22" s="7">
         <v>1.2</v>
       </c>
-      <c r="L22" s="16">
+      <c r="L22" s="23">
         <f>E$9*C$22</f>
-        <v>4.5714285714285712</v>
-      </c>
-      <c r="M22" s="16">
+        <v>4571.4285714285716</v>
+      </c>
+      <c r="M22" s="23">
         <f>F$9*C21</f>
-        <v>4</v>
-      </c>
-      <c r="N22" s="17">
+        <v>4000</v>
+      </c>
+      <c r="N22" s="24">
         <f>L22+M22</f>
-        <v>8.5714285714285712</v>
-      </c>
-      <c r="O22" s="16">
+        <v>8571.4285714285725</v>
+      </c>
+      <c r="O22" s="23">
         <f>G$9*K22</f>
-        <v>14.399999999999999</v>
+        <v>14400</v>
       </c>
       <c r="P22" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q22" s="20">
         <f>O24</f>
-        <v>25.2</v>
+        <v>25200</v>
       </c>
       <c r="R22" s="5">
         <f>K22/Q$24</f>
         <v>1.2244897959183674</v>
       </c>
-      <c r="S22" s="5">
+      <c r="S22" s="19">
         <f>G$9*R22</f>
-        <v>14.693877551020408</v>
-      </c>
-      <c r="T22" s="5">
+        <v>14693.877551020409</v>
+      </c>
+      <c r="T22" s="19">
         <f>S22-N22</f>
-        <v>6.1224489795918373</v>
+        <v>6122.4489795918362</v>
       </c>
       <c r="U22" s="3">
         <f>T22/N22</f>
-        <v>0.71428571428571441</v>
-      </c>
-    </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.4">
+        <v>0.71428571428571408</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>2</v>
       </c>
@@ -2382,25 +2563,25 @@
         <f>R17</f>
         <v>0.8571428571428571</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="20">
         <f>E$10*C$22</f>
-        <v>9.1428571428571423</v>
-      </c>
-      <c r="E23" s="3">
+        <v>9142.8571428571431</v>
+      </c>
+      <c r="E23" s="20">
         <f>F$10*C$21</f>
-        <v>2</v>
-      </c>
-      <c r="F23" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F23" s="20">
         <f>D23+E23</f>
-        <v>11.142857142857142</v>
-      </c>
-      <c r="G23" s="3">
+        <v>11142.857142857143</v>
+      </c>
+      <c r="G23" s="20">
         <f>F$10-E23</f>
-        <v>2</v>
-      </c>
-      <c r="H23" s="5">
+        <v>2000</v>
+      </c>
+      <c r="H23" s="19">
         <f>F23+G23</f>
-        <v>13.142857142857142</v>
+        <v>13142.857142857143</v>
       </c>
       <c r="J23" s="15">
         <f>G23/F23</f>
@@ -2409,118 +2590,129 @@
       <c r="K23" s="7">
         <v>0.9</v>
       </c>
-      <c r="L23" s="16">
+      <c r="L23" s="23">
         <f>E$10*C$22</f>
-        <v>9.1428571428571423</v>
-      </c>
-      <c r="M23" s="16">
+        <v>9142.8571428571431</v>
+      </c>
+      <c r="M23" s="23">
         <f>F$10*K21</f>
-        <v>2</v>
-      </c>
-      <c r="N23" s="17">
+        <v>2000</v>
+      </c>
+      <c r="N23" s="24">
         <f>L23+M23</f>
-        <v>11.142857142857142</v>
-      </c>
-      <c r="O23" s="16">
+        <v>11142.857142857143</v>
+      </c>
+      <c r="O23" s="23">
         <f>G$10*K23</f>
-        <v>10.8</v>
+        <v>10800</v>
       </c>
       <c r="P23" t="s">
         <v>18</v>
       </c>
-      <c r="Q23" s="5">
+      <c r="Q23" s="19">
         <f>H24</f>
-        <v>25.714285714285715</v>
+        <v>25714.285714285717</v>
       </c>
       <c r="R23" s="5">
         <f>K23/Q$24</f>
-        <v>0.91836734693877553</v>
-      </c>
-      <c r="S23" s="5">
+        <v>0.91836734693877564</v>
+      </c>
+      <c r="S23" s="19">
         <f>G$10*R23</f>
-        <v>11.020408163265307</v>
-      </c>
-      <c r="T23" s="5">
+        <v>11020.408163265307</v>
+      </c>
+      <c r="T23" s="19">
         <f>S23-N23</f>
-        <v>-0.12244897959183554</v>
+        <v>-122.44897959183618</v>
       </c>
       <c r="U23" s="3">
         <f>T23/N23</f>
-        <v>-1.0989010989010882E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:25" x14ac:dyDescent="0.4">
+        <v>-1.098901098901094E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="19">
         <f>D23+D22</f>
-        <v>13.714285714285714</v>
-      </c>
-      <c r="E24" s="5">
+        <v>13714.285714285714</v>
+      </c>
+      <c r="E24" s="19">
         <f>E23+E22</f>
-        <v>6</v>
-      </c>
-      <c r="F24" s="5">
+        <v>6000</v>
+      </c>
+      <c r="F24" s="19">
         <f>F23+F22</f>
-        <v>19.714285714285715</v>
-      </c>
-      <c r="G24" s="9">
+        <v>19714.285714285717</v>
+      </c>
+      <c r="G24" s="22">
         <f>G23+G22</f>
-        <v>6</v>
-      </c>
-      <c r="H24">
+        <v>6000</v>
+      </c>
+      <c r="H24" s="19">
         <f>H23+H22</f>
-        <v>25.714285714285715</v>
+        <v>25714.285714285717</v>
       </c>
       <c r="J24" s="15">
         <f>G24/F24</f>
         <v>0.30434782608695649</v>
       </c>
       <c r="K24" s="3"/>
-      <c r="L24" s="17">
+      <c r="L24" s="24">
         <f>L22+L23</f>
-        <v>13.714285714285714</v>
-      </c>
-      <c r="M24" s="17">
+        <v>13714.285714285714</v>
+      </c>
+      <c r="M24" s="24">
         <f>M22+M23</f>
-        <v>6</v>
-      </c>
-      <c r="N24" s="17">
+        <v>6000</v>
+      </c>
+      <c r="N24" s="24">
         <f>N22+N23</f>
-        <v>19.714285714285715</v>
-      </c>
-      <c r="O24" s="17">
+        <v>19714.285714285717</v>
+      </c>
+      <c r="O24" s="24">
         <f>O22+O23</f>
-        <v>25.2</v>
+        <v>25200</v>
       </c>
       <c r="P24" t="s">
         <v>13</v>
       </c>
       <c r="Q24" s="5">
         <f>Q22/Q23</f>
-        <v>0.98</v>
-      </c>
-      <c r="S24" s="3">
+        <v>0.97999999999999987</v>
+      </c>
+      <c r="S24" s="20">
         <f>S22+S23</f>
-        <v>25.714285714285715</v>
-      </c>
-      <c r="T24" s="9">
+        <v>25714.285714285717</v>
+      </c>
+      <c r="T24" s="22">
         <f>T22+T23</f>
-        <v>6.0000000000000018</v>
+        <v>6000</v>
       </c>
       <c r="U24" s="3">
         <f>T24/N24</f>
-        <v>0.3043478260869566</v>
-      </c>
+        <v>0.30434782608695649</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="R13:U13"/>
-    <mergeCell ref="W21:Y21"/>
+    <mergeCell ref="J26:Q26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>